<commit_message>
added a testing folder for spaticott where a possible extension for the latter was tested. basically what's there is a library that can be used by spaticott to connect to tcc services. the two files are done and just need to be cleaned of console logs. next step: creating an extension for node.js to let people create their own tcc services & txmanagers
</commit_message>
<xml_diff>
--- a/testsheet.xlsx
+++ b/testsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15340" yWindow="-220" windowWidth="24800" windowHeight="15660" tabRatio="500"/>
+    <workbookView xWindow="7560" yWindow="-420" windowWidth="24800" windowHeight="15660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="42">
   <si>
     <t>Reservations</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -162,6 +162,30 @@
   </si>
   <si>
     <t>takes too much</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x~~</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>takes too much</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x~~</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -532,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F155"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="D147" sqref="D147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2108,6 +2132,9 @@
       <c r="C118">
         <v>1</v>
       </c>
+      <c r="D118" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119">
@@ -2119,6 +2146,9 @@
       <c r="C119">
         <v>10</v>
       </c>
+      <c r="D119" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120">
@@ -2130,6 +2160,9 @@
       <c r="C120">
         <v>100</v>
       </c>
+      <c r="D120" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121">
@@ -2141,6 +2174,9 @@
       <c r="C121">
         <v>250</v>
       </c>
+      <c r="D121" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122">
@@ -2152,6 +2188,9 @@
       <c r="C122">
         <v>500</v>
       </c>
+      <c r="D122" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123">
@@ -2163,6 +2202,9 @@
       <c r="C123">
         <v>750</v>
       </c>
+      <c r="D123" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124">
@@ -2173,6 +2215,9 @@
       </c>
       <c r="C124">
         <v>1000</v>
+      </c>
+      <c r="D124" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2196,8 +2241,11 @@
       <c r="C128">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:3">
+      <c r="D128" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129">
         <v>1200000</v>
       </c>
@@ -2207,8 +2255,11 @@
       <c r="C129">
         <v>10</v>
       </c>
-    </row>
-    <row r="130" spans="1:3">
+      <c r="D129" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130">
         <v>1200000</v>
       </c>
@@ -2218,8 +2269,11 @@
       <c r="C130">
         <v>100</v>
       </c>
-    </row>
-    <row r="131" spans="1:3">
+      <c r="D130" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131">
         <v>1200000</v>
       </c>
@@ -2229,8 +2283,11 @@
       <c r="C131">
         <v>250</v>
       </c>
-    </row>
-    <row r="132" spans="1:3">
+      <c r="D131" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132">
         <v>1200000</v>
       </c>
@@ -2240,8 +2297,11 @@
       <c r="C132">
         <v>500</v>
       </c>
-    </row>
-    <row r="133" spans="1:3">
+      <c r="D132" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133">
         <v>1200000</v>
       </c>
@@ -2251,8 +2311,11 @@
       <c r="C133">
         <v>750</v>
       </c>
-    </row>
-    <row r="134" spans="1:3">
+      <c r="D133" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134">
         <v>1200000</v>
       </c>
@@ -2262,8 +2325,11 @@
       <c r="C134">
         <v>1000</v>
       </c>
-    </row>
-    <row r="135" spans="1:3">
+      <c r="D134" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135">
         <v>1200000</v>
       </c>
@@ -2273,8 +2339,11 @@
       <c r="C135">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:3">
+      <c r="D135" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136">
         <v>1200000</v>
       </c>
@@ -2284,8 +2353,11 @@
       <c r="C136">
         <v>10</v>
       </c>
-    </row>
-    <row r="137" spans="1:3">
+      <c r="D136" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137">
         <v>1200000</v>
       </c>
@@ -2295,8 +2367,11 @@
       <c r="C137">
         <v>100</v>
       </c>
-    </row>
-    <row r="138" spans="1:3">
+      <c r="D137" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138">
         <v>1200000</v>
       </c>
@@ -2306,8 +2381,11 @@
       <c r="C138">
         <v>250</v>
       </c>
-    </row>
-    <row r="139" spans="1:3">
+      <c r="D138" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139">
         <v>1200000</v>
       </c>
@@ -2317,8 +2395,11 @@
       <c r="C139">
         <v>500</v>
       </c>
-    </row>
-    <row r="140" spans="1:3">
+      <c r="D139" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140">
         <v>1200000</v>
       </c>
@@ -2328,8 +2409,11 @@
       <c r="C140">
         <v>750</v>
       </c>
-    </row>
-    <row r="141" spans="1:3">
+      <c r="D140" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141">
         <v>1200000</v>
       </c>
@@ -2339,8 +2423,11 @@
       <c r="C141">
         <v>1000</v>
       </c>
-    </row>
-    <row r="142" spans="1:3">
+      <c r="D141" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142">
         <v>1200000</v>
       </c>
@@ -2350,8 +2437,11 @@
       <c r="C142">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:3">
+      <c r="D142" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143">
         <v>1200000</v>
       </c>
@@ -2361,8 +2451,11 @@
       <c r="C143">
         <v>10</v>
       </c>
-    </row>
-    <row r="144" spans="1:3">
+      <c r="D143" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144">
         <v>1200000</v>
       </c>
@@ -2372,8 +2465,11 @@
       <c r="C144">
         <v>100</v>
       </c>
-    </row>
-    <row r="145" spans="1:3">
+      <c r="D144" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145">
         <v>1200000</v>
       </c>
@@ -2383,8 +2479,11 @@
       <c r="C145">
         <v>250</v>
       </c>
-    </row>
-    <row r="146" spans="1:3">
+      <c r="D145" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146">
         <v>1200000</v>
       </c>
@@ -2394,8 +2493,11 @@
       <c r="C146">
         <v>500</v>
       </c>
-    </row>
-    <row r="147" spans="1:3">
+      <c r="D146" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147">
         <v>1200000</v>
       </c>
@@ -2406,7 +2508,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:4">
       <c r="A148">
         <v>1200000</v>
       </c>
@@ -2417,7 +2519,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:4">
       <c r="A149">
         <v>1200000</v>
       </c>
@@ -2428,7 +2530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:4">
       <c r="A150">
         <v>1200000</v>
       </c>
@@ -2439,7 +2541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:4">
       <c r="A151">
         <v>1200000</v>
       </c>
@@ -2450,7 +2552,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:4">
       <c r="A152">
         <v>1200000</v>
       </c>
@@ -2461,7 +2563,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:4">
       <c r="A153">
         <v>1200000</v>
       </c>
@@ -2472,7 +2574,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:4">
       <c r="A154">
         <v>1200000</v>
       </c>
@@ -2483,7 +2585,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:4">
       <c r="A155">
         <v>1200000</v>
       </c>
@@ -2495,6 +2597,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>